<commit_message>
MMT Test frame work
</commit_message>
<xml_diff>
--- a/src/main/java/com/MMT/qa/testdata/MMTPassengerDetails.xlsx
+++ b/src/main/java/com/MMT/qa/testdata/MMTPassengerDetails.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>MobileNo</t>
   </si>
@@ -46,13 +46,16 @@
   </si>
   <si>
     <t>MALE</t>
+  </si>
+  <si>
+    <t>8898938122</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +78,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -104,11 +113,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -393,7 +403,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,11 +440,11 @@
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2">
-        <v>8898938122</v>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Frame Work Design for MMT
</commit_message>
<xml_diff>
--- a/src/main/java/com/MMT/qa/testdata/MMTPassengerDetails.xlsx
+++ b/src/main/java/com/MMT/qa/testdata/MMTPassengerDetails.xlsx
@@ -27,28 +27,28 @@
     <t>Email</t>
   </si>
   <si>
-    <t>vishalgupta.2711@gmail.com</t>
-  </si>
-  <si>
     <t>FirstAndMiddleName</t>
   </si>
   <si>
     <t>LastName</t>
   </si>
   <si>
-    <t>VishalRavindra</t>
-  </si>
-  <si>
-    <t>Gupta</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
     <t>MALE</t>
   </si>
   <si>
-    <t>8898938122</t>
+    <t>Vamsi</t>
+  </si>
+  <si>
+    <t>Yellamraju</t>
+  </si>
+  <si>
+    <t>7406683580</t>
+  </si>
+  <si>
+    <t>yvamsipanda9@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,13 +418,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -435,19 +435,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>